<commit_message>
general task no change, PDF Generator all input taken from CSV
</commit_message>
<xml_diff>
--- a/PDFGenerator/PDF/students.xlsx
+++ b/PDFGenerator/PDF/students.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Candidate</t>
-  </si>
-  <si>
     <t>anna</t>
   </si>
   <si>
@@ -117,13 +114,31 @@
   </si>
   <si>
     <t>hart@gmail.com</t>
+  </si>
+  <si>
+    <t>Father Name</t>
+  </si>
+  <si>
+    <t>Mother Name</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Nationality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +153,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,9 +181,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,20 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,228 +499,529 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(111111,999999)</f>
+        <v>177167</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>215</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>124567895</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Mithu","Rashid","Mojnu","Kholil","Rahim")</f>
+        <v>Mithu</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Mithi","Rashida","Morjina","Kholila","Rahima")</f>
+        <v>Morjina</v>
+      </c>
+      <c r="G2" s="3">
+        <f ca="1">DATE(RANDBETWEEN(1995,2018),RANDBETWEEN(1,12),RANDBETWEEN(1,31))</f>
+        <v>42404</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Mirpur, Dhaka","Dhanmondi, Dhaka","College Road, Habiganj","CNB, Rajhshahi","Narail")</f>
+        <v>Mirpur, Dhaka</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Islam","Hindu","Christian","Buddhism","No Religion")</f>
+        <v>Christian</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Bangladesh","India","Pakistan","Nepal","Bhutan")</f>
+        <v>Nepal</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>216</v>
+        <f t="shared" ref="A3:A14" ca="1" si="0">RANDBETWEEN(111111,999999)</f>
+        <v>813028</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>124567896</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f t="shared" ref="E3:E14" ca="1" si="1">CHOOSE(RANDBETWEEN(1,5),"Mithu","Rashid","Mojnu","Kholil","Rahim")</f>
+        <v>Rashid</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F14" ca="1" si="2">CHOOSE(RANDBETWEEN(1,5),"Mithi","Rashida","Morjina","Kholila","Rahima")</f>
+        <v>Mithi</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G14" ca="1" si="3">DATE(RANDBETWEEN(1995,2018),RANDBETWEEN(1,12),RANDBETWEEN(1,31))</f>
+        <v>42576</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H14" ca="1" si="4">CHOOSE(RANDBETWEEN(1,5),"Mirpur, Dhaka","Dhanmondi, Dhaka","College Road, Habiganj","CNB, Rajhshahi","Narail")</f>
+        <v>Dhanmondi, Dhaka</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I14" ca="1" si="5">CHOOSE(RANDBETWEEN(1,5),"Islam","Hindu","Christian","Buddhism","No Religion")</f>
+        <v>Buddhism</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J14" ca="1" si="6">CHOOSE(RANDBETWEEN(1,5),"Bangladesh","India","Pakistan","Nepal","Bhutan")</f>
+        <v>Bhutan</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>217</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>538067</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>124567897</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mojnu</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rahima</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>34808</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Mirpur, Dhaka</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>No Religion</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>Bhutan</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>218</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>892111</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>124567898</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Rashid</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rashida</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>34787</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>CNB, Rajhshahi</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Hindu</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>Pakistan</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>219</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>111592</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>124567899</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mojnu</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rashida</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>39169</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Mirpur, Dhaka</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>No Religion</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>220</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>295243</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>124567900</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mithu</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Kholila</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>39932</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Narail</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Christian</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>221</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>470559</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>124567901</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mithu</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rahima</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>37279</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Dhanmondi, Dhaka</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Islam</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>222</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>126536</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>124567902</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mithu</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rashida</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>37192</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Dhanmondi, Dhaka</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Christian</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>223</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>234101</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>124567903</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mojnu</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Morjina</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>37384</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>College Road, Habiganj</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Hindu</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>224</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>844153</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>124567904</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Rahim</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Kholila</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>40535</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>CNB, Rajhshahi</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Hindu</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>225</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>551797</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>124567905</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Mithu</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rashida</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>39560</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>CNB, Rajhshahi</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Christian</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>226</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>705639</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>124567906</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Rahim</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rahima</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>40180</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Mirpur, Dhaka</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Hindu</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>227</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>980890</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>124567907</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Rahim</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Rahima</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>34875</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Mirpur, Dhaka</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>No Religion</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>Nepal</v>
       </c>
     </row>
   </sheetData>
@@ -713,5 +1041,6 @@
     <hyperlink ref="D14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>